<commit_message>
Se validan las preguntas vacias
</commit_message>
<xml_diff>
--- a/myapp/base_de_datos_turismo.xlsx
+++ b/myapp/base_de_datos_turismo.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -663,40 +663,40 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>123456789</t>
+          <t>1005897049</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>hola</t>
+          <t>quiero hacer deportes peligrosos</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>¡Bienvenido/a a Kofi, tu guía virtual del Quindío! ¿Tienes curiosidad por conocer nuestros paisajes exuberantes, nuestra cultura cafetera o nuestras actividades emocionantes? Estoy aquí para ayudarte.</t>
+          <t>El Valle del Cócora: Este es un lugar perfecto para hacer canopy y tirolesa, donde puedes disfrutar de las vistas de los paisajes montañosos y los valles verdes.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>saludo</t>
+          <t>deportes_extremos</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>cristian</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>méxico</t>
+          <t>colombia</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>ciudad de méxico</t>
+          <t>armenia</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -708,40 +708,40 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>123456789</t>
+          <t>1005897049</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>tienes museos</t>
+          <t>sitios del quindio para explorar</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>¡Amigo turista, estás en el lugar indicado para saborear lo mejor del Quindío! Te sugiero visitar el restaurante 'El Fogón de Doña Rosa' en Filandia. Allí encontrarás delicias como el mondongo quindiano y las empanadas de pipián. Es un lugar donde la tradición y la buena comida se fusionan en cada plato. ¡No te lo puedes perder!</t>
+          <t>¡Bienvenido, amigo viajero! Salento es un destino que te enamorará con sus calles coloridas y su atmósfera única. Te invito a explorar sus encantos naturales y a disfrutar de la hospitalidad de nuestra gente.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>restaurantes</t>
+          <t>sitios</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Juan Pérez</t>
+          <t>cristian</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>méxico</t>
+          <t>colombia</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>ciudad de méxico</t>
+          <t>armenia</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -758,17 +758,17 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>deseo desayunar</t>
+          <t>hola</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>¡Bienvenido a nuestro paraíso gastronómico, mi amigo! Si buscas una experiencia culinaria única, te sugiero el restaurante 'El Mirador' en el Parque Nacional Natural Los Nevados. Podrás degustar platos gourmet con ingredientes frescos y locales, mientras disfrutas de las impresionantes vistas de nuestros paisajes montañosos. ¡Será una experiencia inolvidable para tus sentidos!</t>
+          <t>¡Bienvenido/a a Kofi, tu guía virtual del Quindío! ¿Tienes curiosidad por conocer nuestros paisajes exuberantes, nuestra cultura cafetera o nuestras actividades emocionantes? Estoy aquí para ayudarte.</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>restaurantes</t>
+          <t>saludo</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -803,12 +803,12 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>chao</t>
+          <t>tienes museos</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>¡Por supuesto, mi estimado visitante! Te sugiero probar el restaurante 'Sabor Quindiano'. Ahí encontrarás los sabores auténticos de nuestra tierra, como el inigualable sancocho de gallina y las arepas de chócolo. Está ubicado en el centro de Armenia, en la Calle 14, justo al lado de la Plaza de Bolívar. Te sentirás como en casa, disfrutando de nuestra deliciosa gastronomía.</t>
+          <t>¡Amigo turista, estás en el lugar indicado para saborear lo mejor del Quindío! Te sugiero visitar el restaurante 'El Fogón de Doña Rosa' en Filandia. Allí encontrarás delicias como el mondongo quindiano y las empanadas de pipián. Es un lugar donde la tradición y la buena comida se fusionan en cada plato. ¡No te lo puedes perder!</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -835,6 +835,1716 @@
         </is>
       </c>
       <c r="I9" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>deseo desayunar</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>¡Bienvenido a nuestro paraíso gastronómico, mi amigo! Si buscas una experiencia culinaria única, te sugiero el restaurante 'El Mirador' en el Parque Nacional Natural Los Nevados. Podrás degustar platos gourmet con ingredientes frescos y locales, mientras disfrutas de las impresionantes vistas de nuestros paisajes montañosos. ¡Será una experiencia inolvidable para tus sentidos!</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Juan Pérez</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>25</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>méxico</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>ciudad de méxico</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>chao</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>¡Por supuesto, mi estimado visitante! Te sugiero probar el restaurante 'Sabor Quindiano'. Ahí encontrarás los sabores auténticos de nuestra tierra, como el inigualable sancocho de gallina y las arepas de chócolo. Está ubicado en el centro de Armenia, en la Calle 14, justo al lado de la Plaza de Bolívar. Te sentirás como en casa, disfrutando de nuestra deliciosa gastronomía.</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Juan Pérez</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>25</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>méxico</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>ciudad de méxico</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>¡Hola, bienvenido/a! Soy Kofi, el chatbot con sabor a café y raíces quindianas. ¿En qué puedo ayudarte a descubrir sobre nuestra hermosa región del Quindío?</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>saludo</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>20</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>hola kofi</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>¡Hola, hola! Aquí está Kofi, el chatbot lleno de alegría y hospitalidad quindiana. ¿Necesitas recomendaciones, información o consejos para disfrutar al máximo tu visita al Quindío?</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>saludo</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>20</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>sitios en el quindio</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>¡Claro que sí, mi compadre viajero! La Casa Museo Cipriano Echeverri en Calarcá es un lugar que te permite sumergirte en nuestras raíces y conocer la historia de nuestra región. Y para relajarte, te sugiero disfrutar de las aguas termales de Santa Rosa de Cabal, un verdadero deleite para el cuerpo y el espíritu.</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>sitios</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>20</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>que museos se pueden encontrar en el quindio</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>¡Ay, mi vecino! Te recomiendo visitar el Museo del Oro Quimbaya, donde podrás maravillarte con las increíbles piezas de la antigua cultura quimbaya. Está ubicado en la ciudad de Armenia, la capital cafetera del Quindío.</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>museos</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>20</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>quiero comer algo antes, que lugar para comer me recomiendas</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>¡Hola, amigo/a! Soy Kofi, el chatbot con el acento quindiano. ¿Quieres saber qué lugares visitar, dónde probar nuestra deliciosa gastronomía o qué actividades turísticas te esperan en el Quindío?</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>saludo</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>20</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>quiero comer algo</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>¡Claro, mi amigo! Si quieres degustar los sabores tradicionales de nuestra región, te recomiendo el restaurante 'La Cocina de la Abuela', en Salento. Allí podrás disfrutar de platos como el ají de pollo y el famoso tamal quindiano. Además, el ambiente rústico y acogedor te hará sentir como parte de nuestra familia quindiana.</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>20</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>que deportes extremos se pueden practicar en el quindio</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Río Verde: Este río es otro lugar popular para hacer rafting y kayak. Aquí también puedes encontrar opciones para hacer canyoning y puenting.</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>deportes_extremos</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>20</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>deportes extremos</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>Circasia: Este es un pueblo ubicado en el centro del Quindío, que ofrece opciones para hacer ciclismo de montaña y senderismo.</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>deportes_extremos</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>20</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>lugar para desayunar</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>¡Amigo turista, estás en el lugar indicado para saborear lo mejor del Quindío! Te sugiero visitar el restaurante 'El Fogón de Doña Rosa' en Filandia. Allí encontrarás delicias como el mondongo quindiano y las empanadas de pipián. Es un lugar donde la tradición y la buena comida se fusionan en cada plato. ¡No te lo puedes perder!</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Andres</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>20</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>medellin</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>necesito un lugar para comer en familia</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>¡Por supuesto, mi estimado visitante! Te sugiero probar el restaurante 'Sabor Quindiano'. Ahí encontrarás los sabores auténticos de nuestra tierra, como el inigualable sancocho de gallina y las arepas de chócolo. Está ubicado en el centro de Armenia, en la Calle 14, justo al lado de la Plaza de Bolívar. Te sentirás como en casa, disfrutando de nuestra deliciosa gastronomía.</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>Alfredo</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>60</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>bogota</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>a que museo podemos ir</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>¡Claro, viajero curioso! En el Quindío, podrás maravillarte con nuestros monumentos llenos de historia y cultura. Te recomiendo visitar el monumento a la Cultura Cafetera, ubicado en el Parque Nacional del Café, en el municipio de Montenegro. Aquí podrás aprender sobre la importancia del café en nuestra región. También puedes explorar el monumento a la Colonización, ubicado en el municipio de Armenia, en la Avenida Centenario. Este monumento rinde homenaje a los valientes colonos que forjaron estas tierras. ¡Prepara tu cámara y descubre la grandeza de nuestros monumentos!</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>monumentos</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>Alfredo</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>60</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>bogota</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>tienes museos</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>¡Mi gente bonita! Si te apasiona la cultura cafetera, te sugiero visitar el Parque Nacional del Café. Es un lugar emblemático donde aprenderás sobre el cultivo del café, podrás disfrutar de atracciones y montañas rusas, y vivirás la experiencia cafetera de principio a fin.</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>museos</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Alfredo</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>60</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>bogota</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>que monumento hay en el quindio</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>¡Hola, amante de la historia! El Quindío alberga monumentos que narran nuestro pasado y nuestra identidad. Te sugiero visitar el monumento al Pensador Quindiano, ubicado en el Parque de la Vida, en el municipio de Armenia. Esta estatua representa el espíritu intelectual y reflexivo de nuestra gente. También puedes explorar el monumento a los Fundadores, ubicado en el Parque Los Fundadores, también en el municipio de Armenia. Este monumento es un tributo a aquellos visionarios que hicieron posible el desarrollo de nuestra región. ¡Déjate llevar por la historia de nuestros monumentos y conoce más sobre nuestra cultura!</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>monumentos</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>Alfredo</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>60</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>bogota</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>tienen murales?</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>¡Hola, amante de la historia! El Quindío alberga monumentos que narran nuestro pasado y nuestra identidad. Te sugiero visitar el monumento al Pensador Quindiano, ubicado en el Parque de la Vida, en el municipio de Armenia. Esta estatua representa el espíritu intelectual y reflexivo de nuestra gente. También puedes explorar el monumento a los Fundadores, ubicado en el Parque Los Fundadores, también en el municipio de Armenia. Este monumento es un tributo a aquellos visionarios que hicieron posible el desarrollo de nuestra región. ¡Déjate llevar por la historia de nuestros monumentos y conoce más sobre nuestra cultura!</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>monumentos</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>Alfredo</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>60</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>bogota</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>quiero visitar un museo</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>¡Claro, viajero curioso! En el Quindío, podrás maravillarte con nuestros monumentos llenos de historia y cultura. Te recomiendo visitar el monumento a la Cultura Cafetera, ubicado en el Parque Nacional del Café, en el municipio de Montenegro. Aquí podrás aprender sobre la importancia del café en nuestra región. También puedes explorar el monumento a la Colonización, ubicado en el municipio de Armenia, en la Avenida Centenario. Este monumento rinde homenaje a los valientes colonos que forjaron estas tierras. ¡Prepara tu cámara y descubre la grandeza de nuestros monumentos!</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>monumentos</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Mercedes</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>56</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>barranquilla</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>que monumentos hay en el quindio</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>¡Claro, viajero curioso! En el Quindío, podrás maravillarte con nuestros monumentos llenos de historia y cultura. Te recomiendo visitar el monumento a la Cultura Cafetera, ubicado en el Parque Nacional del Café, en el municipio de Montenegro. Aquí podrás aprender sobre la importancia del café en nuestra región. También puedes explorar el monumento a la Colonización, ubicado en el municipio de Armenia, en la Avenida Centenario. Este monumento rinde homenaje a los valientes colonos que forjaron estas tierras. ¡Prepara tu cámara y descubre la grandeza de nuestros monumentos!</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>monumentos</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>Mercedes</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>56</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>barranquilla</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>deportes extremos</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Río La Vieja: Este río es un lugar perfecto para hacer rafting y kayak. Hay varios operadores turísticos que ofrecen tours y equipos.</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>deportes_extremos</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Raul</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>23</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>cali</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>necesito un restaurante</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>¡Por supuesto, mi estimado visitante! Te sugiero probar el restaurante 'Sabor Quindiano'. Ahí encontrarás los sabores auténticos de nuestra tierra, como el inigualable sancocho de gallina y las arepas de chócolo. Está ubicado en el centro de Armenia, en la Calle 14, justo al lado de la Plaza de Bolívar. Te sentirás como en casa, disfrutando de nuestra deliciosa gastronomía.</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Raul</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>23</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>cali</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>¡Saludos desde el Quindío! Soy Kofi, el chatbot listo para mostrarte la magia de nuestra región cafetera. ¿En qué puedo orientarte para que disfrutes al máximo tu estadía aquí?</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>saludo</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Marta</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>74</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>cartagena</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>necesito un museo</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>¡Saludos, amigacho! Si te gusta la historia colonial, te recomiendo el Museo Quimbaya Colonial en Salento. Allí podrás apreciar muebles antiguos, vestimenta tradicional y conocer detalles fascinantes de nuestra herencia quindiana.</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>museos</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Marta</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>74</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>cartagena</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>deportes extremos</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>La Tebaida: Este es un pueblo ubicado en el centro del Quindío, que ofrece opciones para hacer ciclismo de montaña y senderismo.</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>deportes_extremos</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>15</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>necesito un lugar donde almorzar</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>¡Bienvenido a nuestro paraíso gastronómico, mi amigo! Si buscas una experiencia culinaria única, te sugiero el restaurante 'El Mirador' en el Parque Nacional Natural Los Nevados. Podrás degustar platos gourmet con ingredientes frescos y locales, mientras disfrutas de las impresionantes vistas de nuestros paisajes montañosos. ¡Será una experiencia inolvidable para tus sentidos!</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>15</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>sitios para explorar</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>¡Así es, mi amigo explorador! Quimbaya es un destino que te sorprenderá con su autenticidad y su riqueza cultural. Y si eres amante de la naturaleza, te invito a explorar el Parque Nacional Natural Los Nevados, un lugar que te ofrece paisajes impresionantes y la oportunidad de estar en contacto con la flora y fauna de nuestra región.</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>sitios</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Daniel</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>15</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>colombia</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>armenia</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>hola kofi</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>¡Hola, amigo/a! Soy Kofi, el chatbot con el acento quindiano. ¿Quieres saber qué lugares visitar, dónde probar nuestra deliciosa gastronomía o qué actividades turísticas te esperan en el Quindío?</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>saludo</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Tatiana</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>68</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>españa</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>barcelona</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>un lugar donde almorzar con la familia</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>¡Hola, mi estimado visitante! Si estás en Quimbaya, te recomiendo el restaurante 'El Rancherito'. Allí podrás disfrutar de la auténtica comida quindiana, como el famoso ajiaco y el suculento lechón asado. Además, el ambiente familiar y cálido te hará sentir como en casa, rodeado de nuestras hermosas montañas.</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Tatiana</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>68</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>españa</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>barcelona</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>un museo interesante para visitar</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>¡Ay, mi vecino! Te recomiendo visitar el Museo del Oro Quimbaya, donde podrás maravillarte con las increíbles piezas de la antigua cultura quimbaya. Está ubicado en la ciudad de Armenia, la capital cafetera del Quindío.</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>museos</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Tatiana</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>68</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>españa</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>barcelona</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>que monumentos hay en el quindio</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>¡Hola, amante de la historia! El Quindío alberga monumentos que narran nuestro pasado y nuestra identidad. Te sugiero visitar el monumento al Pensador Quindiano, ubicado en el Parque de la Vida, en el municipio de Armenia. Esta estatua representa el espíritu intelectual y reflexivo de nuestra gente. También puedes explorar el monumento a los Fundadores, ubicado en el Parque Los Fundadores, también en el municipio de Armenia. Este monumento es un tributo a aquellos visionarios que hicieron posible el desarrollo de nuestra región. ¡Déjate llevar por la historia de nuestros monumentos y conoce más sobre nuestra cultura!</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>monumentos</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Tatiana</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>68</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>españa</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>barcelona</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>gracias, chao</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>¡Buen viaje, queridos viajeros! Siempre tendrán un lugar especial en el corazón del Quindío.</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>despedida</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Tatiana</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>68</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>españa</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>barcelona</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>femenino</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>¡Hola! Soy Kofi, el chatbot quindiano con el orgullo de nuestra tierra en cada palabra. ¿Necesitas información sobre nuestros pueblos pintorescos, nuestros parques naturales o nuestras tradiciones culturales?</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>saludo</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Nicolas</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>68</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>buenos aires</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>un lugar donde almorzar</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>¡Por supuesto, mi estimado visitante! Te sugiero probar el restaurante 'Sabor Quindiano'. Ahí encontrarás los sabores auténticos de nuestra tierra, como el inigualable sancocho de gallina y las arepas de chócolo. Está ubicado en el centro de Armenia, en la Calle 14, justo al lado de la Plaza de Bolívar. Te sentirás como en casa, disfrutando de nuestra deliciosa gastronomía.</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Nicolas</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>68</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>buenos aires</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>que monumentos hay en el quindio</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>¡Hola, amante de la historia! El Quindío alberga monumentos que narran nuestro pasado y nuestra identidad. Te sugiero visitar el monumento al Pensador Quindiano, ubicado en el Parque de la Vida, en el municipio de Armenia. Esta estatua representa el espíritu intelectual y reflexivo de nuestra gente. También puedes explorar el monumento a los Fundadores, ubicado en el Parque Los Fundadores, también en el municipio de Armenia. Este monumento es un tributo a aquellos visionarios que hicieron posible el desarrollo de nuestra región. ¡Déjate llevar por la historia de nuestros monumentos y conoce más sobre nuestra cultura!</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>monumentos</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Nicolas</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>68</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>buenos aires</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>que museos hay en el quindio</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>¡Ay, mi vecino! Te recomiendo visitar el Museo del Oro Quimbaya, donde podrás maravillarte con las increíbles piezas de la antigua cultura quimbaya. Está ubicado en la ciudad de Armenia, la capital cafetera del Quindío.</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>museos</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Nicolas</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>68</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>buenos aires</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>chao</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>¡Adiós, mi gente hermosa! Que la brisa cafetera los acompañe siempre en su camino.</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>despedida</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Nicolas</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>68</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>buenos aires</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>hola</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>¡Hola, hola! Aquí está Kofi, el chatbot lleno de alegría y hospitalidad quindiana. ¿Necesitas recomendaciones, información o consejos para disfrutar al máximo tu visita al Quindío?</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>saludo</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>Nicolas</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>68</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>buenos aires</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>que deportes extremos hay en el quindio</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>El Valle del Cócora: Este es un lugar perfecto para hacer canopy y tirolesa, donde puedes disfrutar de las vistas de los paisajes montañosos y los valles verdes.</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>deportes_extremos</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>Nicolas</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>68</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>buenos aires</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>masculino</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>que actividades en la naturaleza hay en el quindio</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>¡Hola! Una actividad imperdible en el Quindío es el senderismo en el Parque Nacional Natural Tatamá. Aquí podrás disfrutar de increíbles vistas panorámicas y descubrir una gran variedad de flora y fauna. Además, te recomiendo realizar pesca deportiva en nuestros ríos y embalses, una actividad relajante y gratificante.</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Actividades al aire libre</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Nicolas</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>68</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>argentina</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>buenos aires</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
         <is>
           <t>masculino</t>
         </is>

</xml_diff>